<commit_message>
Fixed bug by renaming transect_chl_final to api_chl_final
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-chl-transect/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93614E1F-2CDF-E44B-AA7D-30A1BDE3707A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{CF3B6C10-564E-6C47-BF90-881FFD30946E}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="CustomUnits" sheetId="4" r:id="rId5"/>
     <sheet name="StationData" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="130">
   <si>
     <t>attributeName</t>
   </si>
@@ -255,9 +254,6 @@
   </si>
   <si>
     <t>Missing value</t>
-  </si>
-  <si>
-    <t>attribute</t>
   </si>
   <si>
     <t>code</t>
@@ -434,7 +430,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -805,20 +801,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300E580E-9872-3C47-9F26-CB26D2AA2A1F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -841,62 +837,62 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
         <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
@@ -905,12 +901,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
         <v>65</v>
@@ -919,12 +915,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
         <v>65</v>
@@ -933,12 +929,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
         <v>65</v>
@@ -947,59 +943,59 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>65</v>
@@ -1008,18 +1004,18 @@
         <v>70</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>65</v>
@@ -1028,18 +1024,18 @@
         <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>65</v>
@@ -1048,18 +1044,18 @@
         <v>70</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>65</v>
@@ -1068,18 +1064,18 @@
         <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>65</v>
@@ -1088,18 +1084,18 @@
         <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>65</v>
@@ -1108,18 +1104,18 @@
         <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>65</v>
@@ -1128,58 +1124,58 @@
         <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" t="s">
         <v>102</v>
-      </c>
-      <c r="F21" t="s">
-        <v>103</v>
       </c>
       <c r="G21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" t="s">
         <v>102</v>
-      </c>
-      <c r="F22" t="s">
-        <v>103</v>
       </c>
       <c r="G22" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" t="s">
         <v>124</v>
-      </c>
-      <c r="B23" t="s">
-        <v>125</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>66</v>
@@ -1191,82 +1187,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A68FBC6-3BC0-7445-978E-4E892796C0C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
         <v>127</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1275,16 +1269,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE34D23-6A2F-1B40-8E13-5B7029FB5DC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1316,7 +1310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1348,21 +1342,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
         <v>86</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" t="s">
         <v>88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>89</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1377,21 +1371,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" t="s">
         <v>84</v>
-      </c>
-      <c r="F4" t="s">
-        <v>85</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1406,21 +1400,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
         <v>80</v>
       </c>
-      <c r="C5" t="s">
-        <v>81</v>
-      </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
         <v>90</v>
-      </c>
-      <c r="F5" t="s">
-        <v>91</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
@@ -1435,7 +1429,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1455,7 +1449,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -1467,24 +1461,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
         <v>82</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" t="s">
         <v>84</v>
       </c>
-      <c r="F7" t="s">
-        <v>85</v>
-      </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -1496,24 +1490,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
         <v>86</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" t="s">
         <v>88</v>
       </c>
-      <c r="F8" t="s">
-        <v>89</v>
-      </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1525,7 +1519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1548,7 +1542,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1571,7 +1565,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1605,31 +1599,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" xr:uid="{3C924EAE-23DB-FC44-B11F-9D8181C4E41B}"/>
-    <hyperlink ref="E7" r:id="rId2" xr:uid="{24B53A03-32B7-DF49-9D8F-2B71008C8660}"/>
-    <hyperlink ref="E8" r:id="rId3" xr:uid="{C5818D4C-9C70-5F48-A0F0-9334950CBDC7}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{0FABF3DD-4E1B-7244-9D0E-225AB4F31104}"/>
-    <hyperlink ref="E3" r:id="rId5" xr:uid="{9CEAE30B-8060-1D4D-8108-82337F334C73}"/>
-    <hyperlink ref="E4" r:id="rId6" xr:uid="{C874D466-F2E8-1641-A655-3BEA04C6C38D}"/>
+    <hyperlink ref="E11" r:id="rId1"/>
+    <hyperlink ref="E7" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
+    <hyperlink ref="E4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF5D68B-26C3-CF4A-AD51-038276905488}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1637,23 +1631,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
@@ -1661,7 +1655,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -1675,30 +1669,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D43B32-8CAF-2745-823B-E8670DAD0CFB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>97</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>98</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>99</v>
-      </c>
-      <c r="E1" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1707,16 +1701,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED5B226-86F5-2347-9E81-22A89849D162}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1739,38 +1733,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
         <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
additional edits to metadata templates
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D2F1CB-1662-4C7A-ABF9-D51CC6863E87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39738C2F-3B62-4112-BDC0-4EC6F4453FB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="138">
   <si>
     <t>attributeName</t>
   </si>
@@ -173,27 +173,6 @@
     <t>replicate</t>
   </si>
   <si>
-    <t>vol_filtered</t>
-  </si>
-  <si>
-    <t>tau_calibration</t>
-  </si>
-  <si>
-    <t>rb</t>
-  </si>
-  <si>
-    <t>ra</t>
-  </si>
-  <si>
-    <t>blank</t>
-  </si>
-  <si>
-    <t>rb_blank</t>
-  </si>
-  <si>
-    <t>ra_blank</t>
-  </si>
-  <si>
     <t>chl</t>
   </si>
   <si>
@@ -212,9 +191,6 @@
     <t>depth</t>
   </si>
   <si>
-    <t>method_sample</t>
-  </si>
-  <si>
     <t>bottle_other_method</t>
   </si>
   <si>
@@ -296,9 +272,6 @@
     <t>Primary production</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -323,9 +296,6 @@
     <t>NaN</t>
   </si>
   <si>
-    <t>milliliter</t>
-  </si>
-  <si>
     <t>kilometer</t>
   </si>
   <si>
@@ -344,9 +314,6 @@
     <t>Phaeophytin concentration</t>
   </si>
   <si>
-    <t>Volume of seawater filtered for each sample</t>
-  </si>
-  <si>
     <t>Method by which the associated sample was processed</t>
   </si>
   <si>
@@ -398,9 +365,6 @@
     <t>MIT-WHOI Joint Program</t>
   </si>
   <si>
-    <t>fd_calibration</t>
-  </si>
-  <si>
     <t>method_contributor</t>
   </si>
   <si>
@@ -456,6 +420,30 @@
   </si>
   <si>
     <t>Morkeski</t>
+  </si>
+  <si>
+    <t>OCE-1743430</t>
+  </si>
+  <si>
+    <t>alternate_sample_id</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>quality_flag</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Distance greater than 2 km from NES-LTER standard station</t>
+  </si>
+  <si>
+    <t>Nearest NES-LTER standard station</t>
+  </si>
+  <si>
+    <t>Distance from sample location to nearest NES-LTER standard station</t>
   </si>
 </sst>
 </file>
@@ -840,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -880,10 +868,10 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -891,10 +879,10 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -902,94 +890,94 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" t="s">
         <v>62</v>
-      </c>
-      <c r="F5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -997,226 +985,134 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
+        <v>131</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>69</v>
+        <v>136</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" t="s">
-        <v>69</v>
-      </c>
       <c r="F18" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="G18" t="s">
-        <v>71</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="G19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" t="s">
-        <v>96</v>
-      </c>
-      <c r="G20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1242,76 +1138,76 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1321,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1395,19 +1291,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1424,19 +1320,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1453,31 +1349,23 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" t="s">
-        <v>85</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="G5" t="s">
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1500,7 +1388,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -1514,22 +1402,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s">
         <v>78</v>
-      </c>
-      <c r="F7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" t="s">
-        <v>86</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -1543,22 +1431,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1572,16 +1460,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" t="s">
-        <v>28</v>
+      <c r="E9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
@@ -1595,16 +1486,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
@@ -1618,23 +1509,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" t="s">
-        <v>35</v>
+      <c r="E11" t="s">
+        <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -1648,13 +1532,20 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" t="s">
+        <v>35</v>
       </c>
       <c r="G12" t="s">
         <v>36</v>
@@ -1666,6 +1557,29 @@
         <v>24</v>
       </c>
       <c r="J12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1673,11 +1587,12 @@
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="E8" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="E3" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{6378A0FE-4823-4C72-AD5C-542B4DE57202}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1704,7 +1619,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1712,7 +1627,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -1720,7 +1635,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -1728,7 +1643,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
@@ -1744,7 +1659,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -1760,18 +1675,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1792,19 +1707,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1732,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1847,39 +1762,39 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated some column header definitions
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39738C2F-3B62-4112-BDC0-4EC6F4453FB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA964CF-12C9-4F09-A70D-F72C371994B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Personnel" sheetId="2" r:id="rId3"/>
     <sheet name="Keywords" sheetId="3" r:id="rId4"/>
     <sheet name="CustomUnits" sheetId="4" r:id="rId5"/>
-    <sheet name="StationData" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="137">
   <si>
     <t>attributeName</t>
   </si>
@@ -293,27 +292,12 @@
     <t>microgramsPerLiter</t>
   </si>
   <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>kilometer</t>
   </si>
   <si>
-    <t>Distance from sample location to nearest station</t>
-  </si>
-  <si>
-    <t>station_distance</t>
-  </si>
-  <si>
-    <t>Nearest station is provided per cruise</t>
-  </si>
-  <si>
     <t>nearest_station</t>
   </si>
   <si>
-    <t>Phaeophytin concentration</t>
-  </si>
-  <si>
     <t>Method by which the associated sample was processed</t>
   </si>
   <si>
@@ -341,12 +325,6 @@
     <t>Identifier for research cruise generally including abbreviation for research vessel and voyage number</t>
   </si>
   <si>
-    <t>Size fraction of the filtered sample</t>
-  </si>
-  <si>
-    <t>Associated niskin from the other method</t>
-  </si>
-  <si>
     <t>project_id</t>
   </si>
   <si>
@@ -413,9 +391,6 @@
     <t>NOAA NODC Data Types Thesaurus</t>
   </si>
   <si>
-    <t>Concentration of chlorophyll-a per unit volume of the water body corresponding to BCO-DMO chl_a SeaBASS Chl and CF mass_concentration_of_ chlorophyll_a_in_sea_water</t>
-  </si>
-  <si>
     <t>Kate</t>
   </si>
   <si>
@@ -440,10 +415,31 @@
     <t>Distance greater than 2 km from NES-LTER standard station</t>
   </si>
   <si>
-    <t>Nearest NES-LTER standard station</t>
-  </si>
-  <si>
     <t>Distance from sample location to nearest NES-LTER standard station</t>
+  </si>
+  <si>
+    <t>Concentration of chlorophyll-a per unit volume of the water body http://vocab.nerc.ac.uk/collection/P01/current/CPHLZZXX/ corresponding to BCO-DMO chl_a SeaBASS Chl and CF mass_concentration_of_ chlorophyll_a_in_sea_water</t>
+  </si>
+  <si>
+    <t>Concentration of phaeopigments per unit volume of the water body</t>
+  </si>
+  <si>
+    <t>NES-LTER standard station nearest to the sample location</t>
+  </si>
+  <si>
+    <t>Alternate identifier for the same sample</t>
+  </si>
+  <si>
+    <t>Associated niskin with samples analyzed by another method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size fraction with filter and when applicable prefilter in micrometers </t>
+  </si>
+  <si>
+    <t>Quality flag provided for a subset of the data</t>
+  </si>
+  <si>
+    <t>postdoctoralResearcher</t>
   </si>
 </sst>
 </file>
@@ -830,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -868,7 +864,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
@@ -879,7 +875,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -890,7 +886,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
@@ -901,13 +897,13 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G5" t="s">
         <v>62</v>
@@ -918,7 +914,7 @@
         <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
         <v>55</v>
@@ -932,7 +928,7 @@
         <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
@@ -946,7 +942,7 @@
         <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
         <v>56</v>
@@ -960,7 +956,7 @@
         <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
         <v>56</v>
@@ -971,10 +967,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>57</v>
@@ -985,7 +981,7 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -993,7 +989,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>123</v>
+      </c>
+      <c r="B12" t="s">
+        <v>132</v>
       </c>
       <c r="C12" t="s">
         <v>54</v>
@@ -1004,7 +1003,7 @@
         <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
@@ -1015,7 +1014,7 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>56</v>
@@ -1024,7 +1023,7 @@
         <v>86</v>
       </c>
       <c r="F14" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G14" t="s">
         <v>63</v>
@@ -1035,7 +1034,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>56</v>
@@ -1044,7 +1043,7 @@
         <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G15" t="s">
         <v>63</v>
@@ -1052,10 +1051,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>57</v>
@@ -1063,44 +1062,47 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
         <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G18" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>135</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>56</v>
@@ -1109,7 +1111,7 @@
         <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G19" t="s">
         <v>63</v>
@@ -1146,68 +1148,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
         <v>111</v>
-      </c>
-      <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
         <v>105</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>112</v>
-      </c>
-      <c r="C7" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1219,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1349,23 +1351,23 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E5" s="2"/>
       <c r="G5" t="s">
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1474,6 +1476,9 @@
       <c r="F9" t="s">
         <v>77</v>
       </c>
+      <c r="G9" t="s">
+        <v>136</v>
+      </c>
       <c r="H9" t="s">
         <v>20</v>
       </c>
@@ -1562,10 +1567,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -1619,7 +1624,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1635,7 +1640,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -1643,7 +1648,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
@@ -1659,7 +1664,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -1675,18 +1680,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1725,79 +1730,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
minor edits to metadata templates XLS
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA964CF-12C9-4F09-A70D-F72C371994B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F754FE-DED3-4323-B82B-842C85311D24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -217,9 +217,6 @@
     <t>dimensionless</t>
   </si>
   <si>
-    <t>No associated bottle from the other method</t>
-  </si>
-  <si>
     <t>Missing value</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>0000-0002-7811-4150</t>
   </si>
   <si>
-    <t>Principal Investigator</t>
-  </si>
-  <si>
     <t>Primary production</t>
   </si>
   <si>
@@ -409,9 +403,6 @@
     <t>quality_flag</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Distance greater than 2 km from NES-LTER standard station</t>
   </si>
   <si>
@@ -440,6 +431,15 @@
   </si>
   <si>
     <t>postdoctoralResearcher</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>No associated niskin from the other method</t>
   </si>
 </sst>
 </file>
@@ -826,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -864,7 +864,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
@@ -875,7 +875,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -886,7 +886,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
@@ -897,16 +897,16 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -914,7 +914,7 @@
         <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
         <v>55</v>
@@ -928,7 +928,7 @@
         <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
@@ -942,7 +942,7 @@
         <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>56</v>
@@ -956,7 +956,7 @@
         <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>56</v>
@@ -967,10 +967,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>57</v>
@@ -981,7 +981,7 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -989,10 +989,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
         <v>54</v>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
@@ -1014,19 +1014,19 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F14" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1034,27 +1034,27 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F15" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>57</v>
@@ -1062,47 +1062,47 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C17" t="s">
         <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>56</v>
@@ -1111,10 +1111,10 @@
         <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1140,76 +1140,76 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
         <v>104</v>
       </c>
-      <c r="B4" t="s">
-        <v>106</v>
-      </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
         <v>98</v>
       </c>
-      <c r="B6" t="s">
-        <v>100</v>
-      </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1293,19 +1293,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
         <v>68</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" t="s">
         <v>70</v>
-      </c>
-      <c r="F3" t="s">
-        <v>71</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1322,19 +1322,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
         <v>72</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" t="s">
         <v>74</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1350,24 +1350,24 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>112</v>
+      <c r="C5" t="s">
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="2"/>
       <c r="G5" t="s">
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1390,7 +1390,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -1404,22 +1404,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" t="s">
         <v>70</v>
       </c>
-      <c r="F7" t="s">
-        <v>71</v>
-      </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -1433,22 +1433,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
         <v>72</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" t="s">
         <v>74</v>
       </c>
-      <c r="F8" t="s">
-        <v>75</v>
-      </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1462,22 +1462,22 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
         <v>66</v>
       </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
         <v>76</v>
       </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
       <c r="G9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
@@ -1567,10 +1567,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -1680,18 +1680,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1712,19 +1712,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised abstract, methods, added ORCID, additional_info
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-chl-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C2D870-1881-4F8D-BCF9-1EC70DF551C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="155">
   <si>
     <t>attributeName</t>
   </si>
@@ -490,12 +491,15 @@
   </si>
   <si>
     <t>Filtered on 20 micron filter with 200 micron prefilter</t>
+  </si>
+  <si>
+    <t>0000-0002-2903-5851</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -873,10 +877,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1204,7 +1208,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1389,11 +1393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1746,6 +1750,9 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
+      <c r="F13" t="s">
+        <v>154</v>
+      </c>
       <c r="G13" t="s">
         <v>36</v>
       </c>
@@ -1761,11 +1768,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
-    <hyperlink ref="E8" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="E9" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -1773,7 +1780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1872,7 +1879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
added additionalInfo as XML node
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-chl-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C2D870-1881-4F8D-BCF9-1EC70DF551C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="159">
   <si>
     <t>attributeName</t>
   </si>
@@ -208,9 +207,6 @@
     <t>meter</t>
   </si>
   <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
     <t>Missing value</t>
   </si>
   <si>
@@ -494,12 +490,27 @@
   </si>
   <si>
     <t>0000-0002-2903-5851</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>quality not evaluated, not available or unknown</t>
+  </si>
+  <si>
+    <t>questionable/suspect</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>missing data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -877,11 +888,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -919,7 +930,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
@@ -930,7 +941,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
@@ -941,7 +952,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
@@ -949,27 +960,27 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="F5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" t="s">
         <v>129</v>
-      </c>
-      <c r="G5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>53</v>
@@ -978,10 +989,10 @@
         <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -989,7 +1000,7 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -998,10 +1009,10 @@
         <v>57</v>
       </c>
       <c r="F7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1009,7 +1020,7 @@
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
         <v>54</v>
@@ -1018,10 +1029,10 @@
         <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1029,7 +1040,7 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
@@ -1038,18 +1049,18 @@
         <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
         <v>55</v>
@@ -1060,7 +1071,7 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
@@ -1068,27 +1079,27 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" t="s">
         <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" t="s">
         <v>55</v>
@@ -1099,19 +1110,19 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1119,27 +1130,27 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
         <v>93</v>
-      </c>
-      <c r="B16" t="s">
-        <v>94</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>55</v>
@@ -1147,59 +1158,50 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17" t="s">
         <v>52</v>
       </c>
       <c r="F17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>129</v>
-      </c>
-      <c r="G19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1208,11 +1210,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1227,164 +1229,219 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
         <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
         <v>96</v>
-      </c>
-      <c r="C5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>153</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1393,10 +1450,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -1468,19 +1525,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" t="s">
         <v>67</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1497,19 +1554,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
         <v>69</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" t="s">
         <v>71</v>
-      </c>
-      <c r="F4" t="s">
-        <v>72</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1526,23 +1583,23 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" s="2"/>
       <c r="G5" t="s">
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1565,7 +1622,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -1579,22 +1636,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
         <v>65</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" t="s">
         <v>67</v>
       </c>
-      <c r="F7" t="s">
-        <v>68</v>
-      </c>
       <c r="G7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -1608,22 +1665,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
         <v>69</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" t="s">
         <v>71</v>
       </c>
-      <c r="F8" t="s">
-        <v>72</v>
-      </c>
       <c r="G8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1637,22 +1694,22 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" t="s">
-        <v>74</v>
-      </c>
       <c r="G9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
@@ -1742,16 +1799,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
         <v>115</v>
       </c>
-      <c r="C13" t="s">
-        <v>116</v>
-      </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G13" t="s">
         <v>36</v>
@@ -1768,11 +1825,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E8" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E9" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -1780,7 +1837,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1802,7 +1859,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1810,7 +1867,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -1818,7 +1875,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -1826,7 +1883,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
@@ -1842,7 +1899,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -1858,18 +1915,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
         <v>113</v>
-      </c>
-      <c r="B10" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1879,7 +1936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1890,19 +1947,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated SMD files, quality flags, metadata
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="174">
   <si>
     <t>attributeName</t>
   </si>
@@ -505,6 +505,51 @@
   </si>
   <si>
     <t>missing data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emily </t>
+  </si>
+  <si>
+    <t>Peacock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diana </t>
+  </si>
+  <si>
+    <t>associate</t>
+  </si>
+  <si>
+    <t>OCE-1655687</t>
+  </si>
+  <si>
+    <t>OCE-1655688</t>
+  </si>
+  <si>
+    <t>OCE-1655689</t>
+  </si>
+  <si>
+    <t>Fontaine</t>
+  </si>
+  <si>
+    <t>kmorkeski@whoi.edu</t>
+  </si>
+  <si>
+    <t>epeacock@whoi.edu</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>McKenzie</t>
+  </si>
+  <si>
+    <t>mary_mckenzie@uri.edu</t>
+  </si>
+  <si>
+    <t>fontained@uri.edu</t>
+  </si>
+  <si>
+    <t>ecrockford@whoi.edu</t>
   </si>
 </sst>
 </file>
@@ -892,7 +937,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1147,10 +1192,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>55</v>
@@ -1158,33 +1203,24 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G17" t="s">
-        <v>119</v>
+        <v>93</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>82</v>
+        <v>123</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
       </c>
       <c r="F18" t="s">
         <v>128</v>
@@ -1195,13 +1231,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1213,7 +1258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1451,13 +1496,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1694,22 +1742,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="G9" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
@@ -1718,18 +1763,21 @@
         <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>160</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="G10" t="s">
         <v>28</v>
@@ -1741,21 +1789,24 @@
         <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>161</v>
+      </c>
+      <c r="C11" t="s">
+        <v>166</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="s">
-        <v>30</v>
+      <c r="E11" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -1764,54 +1815,44 @@
         <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>170</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" t="s">
-        <v>35</v>
+      <c r="E12" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
+      <c r="E13" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="F13" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
@@ -1820,6 +1861,88 @@
         <v>24</v>
       </c>
       <c r="J13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1829,10 +1952,15 @@
     <hyperlink ref="E8" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="E9" r:id="rId5"/>
+    <hyperlink ref="E13" r:id="rId5"/>
+    <hyperlink ref="E16" r:id="rId6"/>
+    <hyperlink ref="E10" r:id="rId7"/>
+    <hyperlink ref="E12" r:id="rId8"/>
+    <hyperlink ref="E11" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
flag negative phaeos, update personnel & methods
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="175">
   <si>
     <t>attributeName</t>
   </si>
@@ -550,6 +550,9 @@
   </si>
   <si>
     <t>ecrockford@whoi.edu</t>
+  </si>
+  <si>
+    <t>0000-0001-9172-6904</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1502,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1804,6 +1807,9 @@
       </c>
       <c r="E11" s="2" t="s">
         <v>172</v>
+      </c>
+      <c r="F11" t="s">
+        <v>174</v>
       </c>
       <c r="G11" t="s">
         <v>162</v>

</xml_diff>

<commit_message>
added OOI personnel info and fixed LTER fundingNumber
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="174">
   <si>
     <t>attributeName</t>
   </si>
@@ -519,15 +519,6 @@
     <t>associate</t>
   </si>
   <si>
-    <t>OCE-1655687</t>
-  </si>
-  <si>
-    <t>OCE-1655688</t>
-  </si>
-  <si>
-    <t>OCE-1655689</t>
-  </si>
-  <si>
     <t>Fontaine</t>
   </si>
   <si>
@@ -553,6 +544,12 @@
   </si>
   <si>
     <t>0000-0001-9172-6904</t>
+  </si>
+  <si>
+    <t>help@oceanobservatories.org</t>
+  </si>
+  <si>
+    <t>OOI CGSN Data Team</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1499,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1633,13 +1630,15 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>106</v>
+      <c r="A5" t="s">
+        <v>173</v>
       </c>
       <c r="D5" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="G5" t="s">
         <v>23</v>
       </c>
@@ -1754,7 +1753,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G9" t="s">
         <v>28</v>
@@ -1766,7 +1765,7 @@
         <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>164</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1780,7 +1779,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G10" t="s">
         <v>28</v>
@@ -1792,7 +1791,7 @@
         <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1800,16 +1799,16 @@
         <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G11" t="s">
         <v>162</v>
@@ -1821,24 +1820,33 @@
         <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>163</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1934,7 +1942,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F16" t="s">
         <v>153</v>
@@ -1964,9 +1972,10 @@
     <hyperlink ref="E12" r:id="rId8"/>
     <hyperlink ref="E11" r:id="rId9"/>
     <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E5" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
better OOI personnel format
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -549,7 +549,7 @@
     <t>help@oceanobservatories.org</t>
   </si>
   <si>
-    <t>OOI CGSN Data Team</t>
+    <t xml:space="preserve">OOI CGSN Data Team   </t>
   </si>
 </sst>
 </file>
@@ -1499,11 +1499,12 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="22.296875" customWidth="1"/>
     <col min="6" max="6" width="17.3984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1630,7 +1631,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>173</v>
       </c>
       <c r="D5" t="s">

</xml_diff>

<commit_message>
added EN649 prefilter & updated personnel roles
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>0000-0001-9620-5382</t>
   </si>
   <si>
-    <t>metadataProvider</t>
-  </si>
-  <si>
     <t>keyword</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
     <t>nearest_station</t>
   </si>
   <si>
-    <t>Method by which the associated sample was processed</t>
-  </si>
-  <si>
     <t>Lowercase letter indicating replicate subsample drawn from the same rosette bottle</t>
   </si>
   <si>
@@ -393,9 +387,6 @@
     <t>Distance from sample location to nearest NES-LTER standard station</t>
   </si>
   <si>
-    <t>Concentration of chlorophyll-a per unit volume of the water body http://vocab.nerc.ac.uk/collection/P01/current/CPHLZZXX/ corresponding to BCO-DMO chl_a SeaBASS Chl and CF mass_concentration_of_ chlorophyll_a_in_sea_water</t>
-  </si>
-  <si>
     <t>Concentration of phaeopigments per unit volume of the water body</t>
   </si>
   <si>
@@ -408,9 +399,6 @@
     <t xml:space="preserve">Size fraction with filter and when applicable prefilter in micrometers </t>
   </si>
   <si>
-    <t>postdoctoralResearcher</t>
-  </si>
-  <si>
     <t>PI</t>
   </si>
   <si>
@@ -516,9 +504,6 @@
     <t xml:space="preserve">Diana </t>
   </si>
   <si>
-    <t>associate</t>
-  </si>
-  <si>
     <t>Fontaine</t>
   </si>
   <si>
@@ -550,6 +535,21 @@
   </si>
   <si>
     <t xml:space="preserve">OOI CGSN Data Team   </t>
+  </si>
+  <si>
+    <t>Method by which the sample was processed</t>
+  </si>
+  <si>
+    <t>Concentration of chlorophyll a per unit volume of the water body http://vocab.nerc.ac.uk/collection/P01/current/CPHLZZXX/ corresponding to BCO-DMO chl_a SeaBASS Chl and CF mass_concentration_of_ chlorophyll_a_in_sea_water</t>
+  </si>
+  <si>
+    <t>graduate Student</t>
+  </si>
+  <si>
+    <t>postdoctoral Researcher</t>
+  </si>
+  <si>
+    <t>metadata Provider</t>
   </si>
 </sst>
 </file>
@@ -937,7 +937,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -972,281 +972,281 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
         <v>124</v>
       </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>128</v>
-      </c>
       <c r="G5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" t="s">
         <v>58</v>
-      </c>
-      <c r="F9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G12" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
         <v>118</v>
       </c>
-      <c r="B19" t="s">
-        <v>120</v>
-      </c>
       <c r="C19" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1274,219 +1274,219 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
         <v>98</v>
       </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
         <v>92</v>
       </c>
-      <c r="B6" t="s">
-        <v>94</v>
-      </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1499,13 +1499,14 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.296875" customWidth="1"/>
     <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="7" max="7" width="14.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1553,7 +1554,7 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F2" t="s">
@@ -1574,19 +1575,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
         <v>64</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" t="s">
         <v>66</v>
-      </c>
-      <c r="F3" t="s">
-        <v>67</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1603,19 +1604,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" t="s">
         <v>70</v>
-      </c>
-      <c r="F4" t="s">
-        <v>71</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1632,25 +1633,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1673,7 +1674,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -1687,22 +1688,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" t="s">
         <v>66</v>
       </c>
-      <c r="F7" t="s">
-        <v>67</v>
-      </c>
       <c r="G7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -1716,22 +1717,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" t="s">
         <v>70</v>
       </c>
-      <c r="F8" t="s">
-        <v>71</v>
-      </c>
       <c r="G8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1754,7 +1755,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G9" t="s">
         <v>28</v>
@@ -1771,16 +1772,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="G10" t="s">
         <v>28</v>
@@ -1797,22 +1798,22 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" t="s">
         <v>171</v>
-      </c>
-      <c r="G11" t="s">
-        <v>162</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -1826,16 +1827,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>
@@ -1852,22 +1853,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
         <v>62</v>
       </c>
-      <c r="C13" t="s">
-        <v>63</v>
-      </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
         <v>72</v>
       </c>
-      <c r="F13" t="s">
-        <v>73</v>
-      </c>
       <c r="G13" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
@@ -1920,7 +1921,7 @@
         <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>173</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
@@ -1934,22 +1935,22 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F16" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>173</v>
       </c>
       <c r="H16" t="s">
         <v>20</v>
@@ -1974,9 +1975,10 @@
     <hyperlink ref="E11" r:id="rId9"/>
     <hyperlink ref="E9" r:id="rId10"/>
     <hyperlink ref="E5" r:id="rId11"/>
+    <hyperlink ref="E2" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1995,82 +1997,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2091,19 +2093,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added keyword and edited methods
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="175">
   <si>
     <t>attributeName</t>
   </si>
@@ -550,13 +550,16 @@
   </si>
   <si>
     <t>metadata Provider</t>
+  </si>
+  <si>
+    <t>organic matter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -578,12 +581,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -613,12 +610,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1157,7 +1154,7 @@
       <c r="B14" t="s">
         <v>170</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D14" t="s">
@@ -1177,7 +1174,7 @@
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D15" t="s">
@@ -1197,7 +1194,7 @@
       <c r="B16" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1208,7 +1205,7 @@
       <c r="B17" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1236,7 +1233,7 @@
       <c r="B19" t="s">
         <v>118</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D19" t="s">
@@ -1498,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1612,7 +1609,7 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>69</v>
       </c>
       <c r="F4" t="s">
@@ -1725,7 +1722,7 @@
       <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>69</v>
       </c>
       <c r="F8" t="s">
@@ -1984,10 +1981,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2004,7 +2001,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B2" t="s">
@@ -2012,7 +2009,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B3" t="s">
@@ -2020,7 +2017,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B4" t="s">
@@ -2028,7 +2025,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B5" t="s">
@@ -2036,7 +2033,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B6" t="s">
@@ -2044,7 +2041,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B7" t="s">
@@ -2052,7 +2049,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B8" t="s">
@@ -2060,18 +2057,26 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edited Organic matter to core research area
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -552,7 +552,7 @@
     <t>metadata Provider</t>
   </si>
   <si>
-    <t>organic matter</t>
+    <t>Organic matter</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +1984,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2017,40 +2017,40 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>40</v>
+      <c r="A6" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>108</v>
+      <c r="A7" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>41</v>
+      <c r="A8" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
update authors and add cruises
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0D74D0-49AD-4297-B5A2-38BC7284D413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="171">
   <si>
     <t>attributeName</t>
   </si>
@@ -108,9 +109,6 @@
     <t>OCE-1655686</t>
   </si>
   <si>
-    <t>E. Taylor</t>
-  </si>
-  <si>
     <t>Crockford</t>
   </si>
   <si>
@@ -126,18 +124,6 @@
     <t>contact</t>
   </si>
   <si>
-    <t>Jaxine</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Wolfe</t>
-  </si>
-  <si>
-    <t>0000-0001-9620-5382</t>
-  </si>
-  <si>
     <t>keyword</t>
   </si>
   <si>
@@ -543,9 +529,6 @@
     <t>Concentration of chlorophyll a per unit volume of the water body http://vocab.nerc.ac.uk/collection/P01/current/CPHLZZXX/ corresponding to BCO-DMO chl_a SeaBASS Chl and CF mass_concentration_of_ chlorophyll_a_in_sea_water</t>
   </si>
   <si>
-    <t>graduate Student</t>
-  </si>
-  <si>
     <t>postdoctoral Researcher</t>
   </si>
   <si>
@@ -553,12 +536,18 @@
   </si>
   <si>
     <t>Organic matter</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>E.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -604,7 +593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -612,8 +601,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -930,7 +918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -969,281 +957,281 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
         <v>48</v>
       </c>
-      <c r="B7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" t="s">
         <v>53</v>
-      </c>
-      <c r="D7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" t="s">
-        <v>124</v>
-      </c>
-      <c r="G7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" t="s">
         <v>53</v>
-      </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>124</v>
-      </c>
-      <c r="G8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" t="s">
         <v>53</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" t="s">
-        <v>124</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" t="s">
         <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="G15" t="s">
         <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" t="s">
-        <v>124</v>
-      </c>
-      <c r="G15" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1252,7 +1240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1271,219 +1259,219 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
         <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
         <v>98</v>
-      </c>
-      <c r="C4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
         <v>90</v>
-      </c>
-      <c r="B6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1492,11 +1480,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1572,19 +1560,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>170</v>
+      </c>
+      <c r="B3" t="s">
+        <v>169</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1601,19 +1589,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" t="s">
-        <v>70</v>
+      <c r="E4" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1629,49 +1614,52 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
+      </c>
+      <c r="F5" t="s">
+        <v>161</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
-        <v>21</v>
+      <c r="E6" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>123</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -1685,22 +1673,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
         <v>63</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" t="s">
         <v>65</v>
       </c>
-      <c r="F7" t="s">
-        <v>66</v>
-      </c>
       <c r="G7" t="s">
-        <v>123</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -1713,49 +1701,49 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>163</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" t="s">
-        <v>70</v>
+        <v>99</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="G8" t="s">
-        <v>123</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>165</v>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
@@ -1769,19 +1757,22 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
@@ -1795,22 +1786,22 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>164</v>
+      <c r="E11" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>166</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>171</v>
+        <v>118</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -1824,19 +1815,19 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
@@ -1850,22 +1841,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
@@ -1879,16 +1870,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>30</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
       </c>
       <c r="H14" t="s">
         <v>20</v>
@@ -1902,23 +1893,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>144</v>
       </c>
       <c r="G15" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
@@ -1930,49 +1920,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F16" t="s">
-        <v>149</v>
-      </c>
-      <c r="G16" t="s">
-        <v>173</v>
-      </c>
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
-    <hyperlink ref="E8" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="E13" r:id="rId5"/>
-    <hyperlink ref="E16" r:id="rId6"/>
-    <hyperlink ref="E10" r:id="rId7"/>
-    <hyperlink ref="E12" r:id="rId8"/>
-    <hyperlink ref="E11" r:id="rId9"/>
-    <hyperlink ref="E9" r:id="rId10"/>
-    <hyperlink ref="E5" r:id="rId11"/>
-    <hyperlink ref="E2" r:id="rId12"/>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E11" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E15" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="E4" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="E12" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="E5" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="E3" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="E8" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="E2" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -1980,10 +1941,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1994,90 +1955,90 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>105</v>
+      <c r="A2" t="s">
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>73</v>
+      <c r="A3" t="s">
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>174</v>
+      <c r="A4" t="s">
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>106</v>
+      <c r="A5" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>107</v>
+      <c r="A6" t="s">
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>40</v>
+      <c r="A7" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>41</v>
+      <c r="A9" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>110</v>
+      <c r="A10" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>110</v>
+      <c r="A11" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2087,7 +2048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2098,19 +2059,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to data table and metadata
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0D74D0-49AD-4297-B5A2-38BC7284D413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85631B09-2ED8-452C-87CA-30CFCACF3B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="173">
   <si>
     <t>attributeName</t>
   </si>
@@ -388,9 +388,6 @@
     <t>PI</t>
   </si>
   <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>No associated niskin from the other method</t>
   </si>
   <si>
@@ -442,9 +439,6 @@
     <t>&gt;5&amp;&lt;200</t>
   </si>
   <si>
-    <t>&gt;20&lt;200</t>
-  </si>
-  <si>
     <t>Filtered on 5 micron filter</t>
   </si>
   <si>
@@ -542,13 +536,25 @@
   </si>
   <si>
     <t>E.</t>
+  </si>
+  <si>
+    <t>0000-0002-2122-0462</t>
+  </si>
+  <si>
+    <t>0000-0003-0194-7282</t>
+  </si>
+  <si>
+    <t>"NA"</t>
+  </si>
+  <si>
+    <t>&gt;20&amp;&lt;200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -571,6 +577,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -589,11 +605,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -604,10 +621,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{124505E1-E4E6-4AF6-BC62-4AAF61C17221}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -922,7 +941,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -990,7 +1009,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
         <v>116</v>
@@ -999,15 +1018,15 @@
         <v>46</v>
       </c>
       <c r="F5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" t="s">
         <v>119</v>
-      </c>
-      <c r="G5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
         <v>81</v>
@@ -1019,7 +1038,7 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="G6" t="s">
         <v>53</v>
@@ -1039,7 +1058,7 @@
         <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
@@ -1059,7 +1078,7 @@
         <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
@@ -1070,7 +1089,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
         <v>48</v>
@@ -1079,7 +1098,7 @@
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="G9" t="s">
         <v>53</v>
@@ -1090,7 +1109,7 @@
         <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
         <v>49</v>
@@ -1112,16 +1131,16 @@
         <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="G12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1140,7 +1159,7 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>48</v>
@@ -1149,7 +1168,7 @@
         <v>75</v>
       </c>
       <c r="F14" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="G14" t="s">
         <v>53</v>
@@ -1169,7 +1188,7 @@
         <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="G15" t="s">
         <v>53</v>
@@ -1177,10 +1196,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>49</v>
@@ -1208,7 +1227,7 @@
         <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="G18" t="s">
         <v>112</v>
@@ -1228,7 +1247,7 @@
         <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="G19" t="s">
         <v>112</v>
@@ -1243,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1336,10 +1355,10 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1347,10 +1366,10 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1358,10 +1377,10 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1369,10 +1388,10 @@
         <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1380,10 +1399,10 @@
         <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1391,10 +1410,10 @@
         <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1402,10 +1421,10 @@
         <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1413,65 +1432,65 @@
         <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1483,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1560,10 +1579,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1572,7 +1591,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1589,16 +1611,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1615,19 +1640,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" t="s">
         <v>159</v>
-      </c>
-      <c r="F5" t="s">
-        <v>161</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
@@ -1702,13 +1727,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D8" t="s">
         <v>99</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
@@ -1815,16 +1840,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="C12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
@@ -1856,7 +1881,7 @@
         <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
@@ -1902,13 +1927,13 @@
         <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
@@ -1979,7 +2004,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
v2 methods edits and end use of join_by_url
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85631B09-2ED8-452C-87CA-30CFCACF3B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A99941A-498F-4C54-8534-9003A6911576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
     <sheet name="CategoricalVariables" sheetId="5" r:id="rId2"/>
     <sheet name="Personnel" sheetId="2" r:id="rId3"/>
-    <sheet name="Keywords" sheetId="3" r:id="rId4"/>
-    <sheet name="CustomUnits" sheetId="4" r:id="rId5"/>
+    <sheet name="cruises" sheetId="6" r:id="rId4"/>
+    <sheet name="Keywords" sheetId="3" r:id="rId5"/>
+    <sheet name="CustomUnits" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="219">
   <si>
     <t>attributeName</t>
   </si>
@@ -361,9 +362,6 @@
     <t>OCE-1743430</t>
   </si>
   <si>
-    <t>alternate_sample_id</t>
-  </si>
-  <si>
     <t>distance</t>
   </si>
   <si>
@@ -400,18 +398,12 @@
     <t>iode_quality_flag</t>
   </si>
   <si>
-    <t>OOI filter identifier</t>
-  </si>
-  <si>
     <t>Depth of sample below sea surface as recorded by CTD</t>
   </si>
   <si>
     <t>IODE Quality Flag primary level</t>
   </si>
   <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
     <t>&gt;0</t>
   </si>
   <si>
@@ -548,13 +540,160 @@
   </si>
   <si>
     <t>&gt;20&amp;&lt;200</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>AR16</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>AR22</t>
+  </si>
+  <si>
+    <t>AR24A</t>
+  </si>
+  <si>
+    <t>AR24B</t>
+  </si>
+  <si>
+    <t>AR24C</t>
+  </si>
+  <si>
+    <t>EN608</t>
+  </si>
+  <si>
+    <t>AR28A</t>
+  </si>
+  <si>
+    <t>AR28B</t>
+  </si>
+  <si>
+    <t>EN617</t>
+  </si>
+  <si>
+    <t>AR31A</t>
+  </si>
+  <si>
+    <t>AR31B</t>
+  </si>
+  <si>
+    <t>AR31C</t>
+  </si>
+  <si>
+    <t>AR32</t>
+  </si>
+  <si>
+    <t>EN627</t>
+  </si>
+  <si>
+    <t>AR34A</t>
+  </si>
+  <si>
+    <t>AR34B</t>
+  </si>
+  <si>
+    <t>EN644</t>
+  </si>
+  <si>
+    <t>AR38</t>
+  </si>
+  <si>
+    <t>AR39A</t>
+  </si>
+  <si>
+    <t>AR39B</t>
+  </si>
+  <si>
+    <t>EN649</t>
+  </si>
+  <si>
+    <t>AR44</t>
+  </si>
+  <si>
+    <t>EN655</t>
+  </si>
+  <si>
+    <t>EN657</t>
+  </si>
+  <si>
+    <t>AR48A</t>
+  </si>
+  <si>
+    <t>AR48B</t>
+  </si>
+  <si>
+    <t>EN661</t>
+  </si>
+  <si>
+    <t>AR52A</t>
+  </si>
+  <si>
+    <t>AR52B</t>
+  </si>
+  <si>
+    <t>EN668</t>
+  </si>
+  <si>
+    <t>AR61A</t>
+  </si>
+  <si>
+    <t>AR61B</t>
+  </si>
+  <si>
+    <t>AR62</t>
+  </si>
+  <si>
+    <t>AR63</t>
+  </si>
+  <si>
+    <t>AT46</t>
+  </si>
+  <si>
+    <t>AR66A</t>
+  </si>
+  <si>
+    <t>AR66B</t>
+  </si>
+  <si>
+    <t>EN685</t>
+  </si>
+  <si>
+    <t>EN687</t>
+  </si>
+  <si>
+    <t>EN688</t>
+  </si>
+  <si>
+    <t>OTZ</t>
+  </si>
+  <si>
+    <t>AR70A</t>
+  </si>
+  <si>
+    <t>AR70B</t>
+  </si>
+  <si>
+    <t>EN695</t>
+  </si>
+  <si>
+    <t>in_version2</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>SMD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -587,6 +726,19 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -596,10 +748,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -610,7 +788,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -622,6 +800,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -938,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1009,24 +1199,24 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
         <v>81</v>
@@ -1038,7 +1228,7 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G6" t="s">
         <v>53</v>
@@ -1058,7 +1248,7 @@
         <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
@@ -1078,7 +1268,7 @@
         <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
@@ -1089,7 +1279,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
         <v>48</v>
@@ -1098,7 +1288,7 @@
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G9" t="s">
         <v>53</v>
@@ -1109,7 +1299,7 @@
         <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
         <v>49</v>
@@ -1128,38 +1318,41 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" t="s">
-        <v>171</v>
-      </c>
-      <c r="G12" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
+        <v>160</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>48</v>
@@ -1168,7 +1361,7 @@
         <v>75</v>
       </c>
       <c r="F14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G14" t="s">
         <v>53</v>
@@ -1176,30 +1369,21 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" t="s">
-        <v>171</v>
-      </c>
-      <c r="G15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>49</v>
@@ -1207,50 +1391,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>49</v>
+        <v>114</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
+        <v>112</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
         <v>111</v>
-      </c>
-      <c r="B19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" t="s">
-        <v>171</v>
-      </c>
-      <c r="G19" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1262,7 +1435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1355,10 +1528,10 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1366,10 +1539,10 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1377,10 +1550,10 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1388,10 +1561,10 @@
         <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1399,10 +1572,10 @@
         <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1410,10 +1583,10 @@
         <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1421,10 +1594,10 @@
         <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1432,65 +1605,65 @@
         <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1579,10 +1752,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1591,10 +1764,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1611,19 +1784,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1640,19 +1813,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
@@ -1727,13 +1900,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
         <v>99</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
@@ -1768,7 +1941,7 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
@@ -1797,7 +1970,7 @@
         <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
@@ -1826,7 +1999,7 @@
         <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -1840,16 +2013,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
@@ -1881,7 +2054,7 @@
         <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
@@ -1927,13 +2100,13 @@
         <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
@@ -1966,6 +2139,572 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33916625-81B4-4982-852A-9AC43A1391EB}">
+  <dimension ref="A1:D44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="10.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="9">
+        <v>201704</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="9">
+        <v>20170902</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="9">
+        <v>20171022</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="9">
+        <v>20180131</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="9">
+        <v>20180404</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="9">
+        <v>20180720</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="9">
+        <v>20181020</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="9">
+        <v>20181112</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="9">
+        <v>20190201</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" s="9">
+        <v>20190414</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="9">
+        <v>20190819</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" s="9">
+        <v>20190920</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="9">
+        <v>20190925</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" s="9">
+        <v>20200201</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B23" s="9">
+        <v>20220605</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="9">
+        <v>20200704</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="9">
+        <v>20201013</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B26" s="9">
+        <v>20201028</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B28" s="9">
+        <v>20210129</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B29" s="9">
+        <v>20210329</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="9">
+        <v>20210716</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B32" s="9">
+        <v>20211026</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B34" s="9">
+        <v>20211117</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B35" s="9">
+        <v>20211126</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" s="9">
+        <v>20220216</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="9">
+        <v>20220408</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B39" s="9">
+        <v>20220713</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B40" s="9">
+        <v>20220729</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" s="9">
+        <v>20220804</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B42" s="9">
+        <v>20221109</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44" s="9">
+        <v>20230111</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -2004,7 +2743,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -2072,7 +2811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>

</xml_diff>

<commit_message>
get updated data and edit metadata
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A99941A-498F-4C54-8534-9003A6911576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6370EBA8-B7B9-44FE-A3EF-52A2B909A86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="218">
   <si>
     <t>attributeName</t>
   </si>
@@ -290,9 +290,6 @@
     <t>project_id</t>
   </si>
   <si>
-    <t>Project associated with the sample collected</t>
-  </si>
-  <si>
     <t>JP</t>
   </si>
   <si>
@@ -515,9 +512,6 @@
     <t>Concentration of chlorophyll a per unit volume of the water body http://vocab.nerc.ac.uk/collection/P01/current/CPHLZZXX/ corresponding to BCO-DMO chl_a SeaBASS Chl and CF mass_concentration_of_ chlorophyll_a_in_sea_water</t>
   </si>
   <si>
-    <t>postdoctoral Researcher</t>
-  </si>
-  <si>
     <t>metadata Provider</t>
   </si>
   <si>
@@ -687,6 +681,9 @@
   </si>
   <si>
     <t>SMD</t>
+  </si>
+  <si>
+    <t>Identifier for project that funded the cruise (or sample when available)</t>
   </si>
 </sst>
 </file>
@@ -1131,7 +1128,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1199,24 +1196,24 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>81</v>
@@ -1228,7 +1225,7 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G6" t="s">
         <v>53</v>
@@ -1248,7 +1245,7 @@
         <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
@@ -1268,7 +1265,7 @@
         <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
@@ -1279,7 +1276,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
         <v>48</v>
@@ -1288,7 +1285,7 @@
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G9" t="s">
         <v>53</v>
@@ -1296,10 +1293,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C10" t="s">
         <v>49</v>
@@ -1321,7 +1318,7 @@
         <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
         <v>49</v>
@@ -1332,7 +1329,7 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>48</v>
@@ -1341,7 +1338,7 @@
         <v>75</v>
       </c>
       <c r="F13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G13" t="s">
         <v>53</v>
@@ -1352,7 +1349,7 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>48</v>
@@ -1361,7 +1358,7 @@
         <v>75</v>
       </c>
       <c r="F14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G14" t="s">
         <v>53</v>
@@ -1369,10 +1366,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>49</v>
@@ -1383,7 +1380,7 @@
         <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>217</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>49</v>
@@ -1394,24 +1391,24 @@
         <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C17" t="s">
         <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>48</v>
@@ -1420,10 +1417,10 @@
         <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1459,35 +1456,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1495,10 +1492,10 @@
         <v>85</v>
       </c>
       <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1506,10 +1503,10 @@
         <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1517,10 +1514,10 @@
         <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1528,10 +1525,10 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1539,10 +1536,10 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1550,10 +1547,10 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1561,10 +1558,10 @@
         <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1572,10 +1569,10 @@
         <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1583,10 +1580,10 @@
         <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1594,10 +1591,10 @@
         <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1605,65 +1602,65 @@
         <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1676,7 +1673,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F4"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1752,10 +1749,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1764,10 +1761,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1784,19 +1781,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
         <v>145</v>
-      </c>
-      <c r="C4" t="s">
-        <v>146</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1813,19 +1810,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>154</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>156</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
@@ -1842,19 +1839,19 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>155</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
@@ -1899,78 +1896,78 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>157</v>
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
+        <v>98</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="G9" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="I9" t="s">
         <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>60</v>
+      <c r="E10" t="s">
+        <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
@@ -1984,22 +1981,22 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>64</v>
+      <c r="E11" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -2013,19 +2010,22 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>153</v>
+      <c r="E12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
@@ -2039,22 +2039,19 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
       <c r="G13" t="s">
-        <v>161</v>
+        <v>27</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
@@ -2091,22 +2088,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s">
         <v>107</v>
-      </c>
-      <c r="C15" t="s">
-        <v>108</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
@@ -2120,17 +2117,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E11" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E11" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E12" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="E7" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="E13" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
     <hyperlink ref="E15" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
     <hyperlink ref="E4" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="E12" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="E5" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="E6" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
     <hyperlink ref="E3" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="E8" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="E9" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
     <hyperlink ref="E2" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2156,546 +2153,546 @@
         <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>85</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" s="9">
         <v>201704</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B3" s="9">
         <v>20170902</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B4" s="9">
         <v>20171022</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B7" s="9">
         <v>20180131</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B8" s="9">
         <v>20180404</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" s="9">
         <v>20180720</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B11" s="9">
         <v>20181020</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B14" s="9">
         <v>20181112</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B15" s="9">
         <v>20190201</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B16" s="9">
         <v>20190414</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B18" s="9">
         <v>20190819</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B19" s="9">
         <v>20190920</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B20" s="9">
         <v>20190925</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B22" s="9">
         <v>20200201</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B23" s="9">
         <v>20220605</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B24" s="9">
         <v>20200704</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B25" s="9">
         <v>20201013</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B26" s="9">
         <v>20201028</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B28" s="9">
         <v>20210129</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B29" s="9">
         <v>20210329</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B31" s="9">
         <v>20210716</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B32" s="9">
         <v>20211026</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B34" s="9">
         <v>20211117</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B35" s="9">
         <v>20211126</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B36" s="9">
         <v>20220216</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B37" s="9">
         <v>20220408</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B39" s="9">
         <v>20220713</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B40" s="9">
         <v>20220729</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D40" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B41" s="9">
         <v>20220804</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B42" s="9">
         <v>20221109</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B44" s="9">
         <v>20230111</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2727,7 +2724,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -2743,7 +2740,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -2751,7 +2748,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -2759,7 +2756,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -2775,7 +2772,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -2791,18 +2788,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
         <v>105</v>
-      </c>
-      <c r="B11" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incorporated api updates and pipes for paired cast/niskin
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6370EBA8-B7B9-44FE-A3EF-52A2B909A86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A17B139-FE85-4419-9E2B-33B17A9993F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="215">
   <si>
     <t>attributeName</t>
   </si>
@@ -374,19 +374,10 @@
     <t>NES-LTER standard station nearest to the sample location</t>
   </si>
   <si>
-    <t>Associated niskin with samples analyzed by another method</t>
-  </si>
-  <si>
     <t xml:space="preserve">Size fraction with filter and when applicable prefilter in micrometers </t>
   </si>
   <si>
     <t>PI</t>
-  </si>
-  <si>
-    <t>No associated niskin from the other method</t>
-  </si>
-  <si>
-    <t>niskin_other_method</t>
   </si>
   <si>
     <t>date_time_utc</t>
@@ -1125,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1196,36 +1187,39 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G5" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G6" t="s">
         <v>53</v>
@@ -1233,10 +1227,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
@@ -1245,7 +1239,7 @@
         <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
@@ -1253,19 +1247,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
         <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
@@ -1273,63 +1267,63 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" t="s">
-        <v>166</v>
-      </c>
-      <c r="G9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
+        <v>156</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>48</v>
@@ -1338,7 +1332,7 @@
         <v>75</v>
       </c>
       <c r="F13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G13" t="s">
         <v>53</v>
@@ -1346,30 +1340,21 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" t="s">
-        <v>166</v>
-      </c>
-      <c r="G14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>214</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>49</v>
@@ -1377,49 +1362,38 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>49</v>
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G16" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
+        <v>111</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" t="s">
-        <v>166</v>
-      </c>
-      <c r="G18" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1525,10 +1499,10 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1536,10 +1510,10 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1547,10 +1521,10 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1558,10 +1532,10 @@
         <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1569,10 +1543,10 @@
         <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1580,10 +1554,10 @@
         <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1591,10 +1565,10 @@
         <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1602,65 +1576,65 @@
         <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1749,10 +1723,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1761,10 +1735,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1781,19 +1755,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1839,19 +1813,19 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
@@ -1926,13 +1900,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D9" t="s">
         <v>98</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G9" t="s">
         <v>23</v>
@@ -1967,7 +1941,7 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
@@ -1996,7 +1970,7 @@
         <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -2025,7 +1999,7 @@
         <v>65</v>
       </c>
       <c r="G12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
@@ -2039,16 +2013,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G13" t="s">
         <v>27</v>
@@ -2097,13 +2071,13 @@
         <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
@@ -2153,29 +2127,29 @@
         <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>85</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B2" s="9">
         <v>201704</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B3" s="9">
         <v>20170902</v>
@@ -2184,12 +2158,12 @@
         <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B4" s="9">
         <v>20171022</v>
@@ -2198,36 +2172,36 @@
         <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B7" s="9">
         <v>20180131</v>
@@ -2236,12 +2210,12 @@
         <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B8" s="9">
         <v>20180404</v>
@@ -2250,24 +2224,24 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B10" s="9">
         <v>20180720</v>
@@ -2276,12 +2250,12 @@
         <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B11" s="9">
         <v>20181020</v>
@@ -2290,36 +2264,36 @@
         <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B14" s="9">
         <v>20181112</v>
@@ -2328,12 +2302,12 @@
         <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B15" s="9">
         <v>20190201</v>
@@ -2342,12 +2316,12 @@
         <v>87</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B16" s="9">
         <v>20190414</v>
@@ -2356,24 +2330,24 @@
         <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B18" s="9">
         <v>20190819</v>
@@ -2382,12 +2356,12 @@
         <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B19" s="9">
         <v>20190920</v>
@@ -2396,12 +2370,12 @@
         <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B20" s="9">
         <v>20190925</v>
@@ -2410,24 +2384,24 @@
         <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B22" s="9">
         <v>20200201</v>
@@ -2436,12 +2410,12 @@
         <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B23" s="9">
         <v>20220605</v>
@@ -2452,7 +2426,7 @@
     </row>
     <row r="24" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B24" s="9">
         <v>20200704</v>
@@ -2461,12 +2435,12 @@
         <v>87</v>
       </c>
       <c r="D24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B25" s="9">
         <v>20201013</v>
@@ -2475,12 +2449,12 @@
         <v>87</v>
       </c>
       <c r="D25" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B26" s="9">
         <v>20201028</v>
@@ -2491,7 +2465,7 @@
     </row>
     <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
@@ -2500,7 +2474,7 @@
     </row>
     <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B28" s="9">
         <v>20210129</v>
@@ -2509,12 +2483,12 @@
         <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B29" s="9">
         <v>20210329</v>
@@ -2525,7 +2499,7 @@
     </row>
     <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
@@ -2534,7 +2508,7 @@
     </row>
     <row r="31" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B31" s="9">
         <v>20210716</v>
@@ -2543,12 +2517,12 @@
         <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B32" s="9">
         <v>20211026</v>
@@ -2559,30 +2533,30 @@
     </row>
     <row r="33" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B34" s="9">
         <v>20211117</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B35" s="9">
         <v>20211126</v>
@@ -2593,7 +2567,7 @@
     </row>
     <row r="36" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B36" s="9">
         <v>20220216</v>
@@ -2602,12 +2576,12 @@
         <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B37" s="9">
         <v>20220408</v>
@@ -2618,30 +2592,30 @@
     </row>
     <row r="38" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B39" s="9">
         <v>20220713</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B40" s="9">
         <v>20220729</v>
@@ -2650,23 +2624,23 @@
         <v>87</v>
       </c>
       <c r="D40" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B41" s="9">
         <v>20220804</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B42" s="9">
         <v>20221109</v>
@@ -2677,7 +2651,7 @@
     </row>
     <row r="43" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
@@ -2686,7 +2660,7 @@
     </row>
     <row r="44" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B44" s="9">
         <v>20230111</v>
@@ -2740,7 +2714,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
edit methods and tidy up script
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A17B139-FE85-4419-9E2B-33B17A9993F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EE98D1-1F85-4E91-B2A5-9158D9C99C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Personnel" sheetId="2" r:id="rId3"/>
     <sheet name="cruises" sheetId="6" r:id="rId4"/>
     <sheet name="Keywords" sheetId="3" r:id="rId5"/>
-    <sheet name="CustomUnits" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="210">
   <si>
     <t>attributeName</t>
   </si>
@@ -237,21 +236,6 @@
   </si>
   <si>
     <t>Primary production</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>unitType</t>
-  </si>
-  <si>
-    <t>parentSI</t>
-  </si>
-  <si>
-    <t>multiplierToSI</t>
-  </si>
-  <si>
-    <t>description</t>
   </si>
   <si>
     <t>filter_size</t>
@@ -1118,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -1157,7 +1141,7 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
@@ -1168,7 +1152,7 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -1179,7 +1163,7 @@
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -1187,10 +1171,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -1199,7 +1183,7 @@
         <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G5" t="s">
         <v>53</v>
@@ -1210,7 +1194,7 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
@@ -1219,7 +1203,7 @@
         <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G6" t="s">
         <v>53</v>
@@ -1230,7 +1214,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
@@ -1239,7 +1223,7 @@
         <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
@@ -1250,7 +1234,7 @@
         <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
         <v>48</v>
@@ -1259,7 +1243,7 @@
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
@@ -1267,10 +1251,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s">
         <v>49</v>
@@ -1281,7 +1265,7 @@
         <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
@@ -1289,10 +1273,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
         <v>49</v>
@@ -1303,16 +1287,16 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G12" t="s">
         <v>53</v>
@@ -1323,16 +1307,16 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G13" t="s">
         <v>53</v>
@@ -1340,10 +1324,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>49</v>
@@ -1351,10 +1335,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>49</v>
@@ -1362,39 +1346,39 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
         <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G17" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1430,211 +1414,211 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
         <v>90</v>
-      </c>
-      <c r="B2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
         <v>92</v>
-      </c>
-      <c r="C4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
         <v>124</v>
-      </c>
-      <c r="C10" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
         <v>125</v>
-      </c>
-      <c r="C11" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
         <v>126</v>
-      </c>
-      <c r="C12" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
         <v>127</v>
-      </c>
-      <c r="C13" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" t="s">
         <v>128</v>
-      </c>
-      <c r="C14" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1723,10 +1707,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1735,10 +1719,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1755,19 +1739,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1813,19 +1797,19 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
@@ -1900,25 +1884,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G9" t="s">
         <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I9" t="s">
         <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1941,7 +1925,7 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
@@ -1970,7 +1954,7 @@
         <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -1999,7 +1983,7 @@
         <v>65</v>
       </c>
       <c r="G12" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
@@ -2013,16 +1997,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G13" t="s">
         <v>27</v>
@@ -2062,22 +2046,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F15" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G15" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
@@ -2113,7 +2097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33916625-81B4-4982-852A-9AC43A1391EB}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2127,546 +2111,546 @@
         <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B2" s="9">
         <v>201704</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="9">
         <v>20170902</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B4" s="9">
         <v>20171022</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B7" s="9">
         <v>20180131</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B8" s="9">
         <v>20180404</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B10" s="9">
         <v>20180720</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B11" s="9">
         <v>20181020</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B14" s="9">
         <v>20181112</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B15" s="9">
         <v>20190201</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B16" s="9">
         <v>20190414</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B18" s="9">
         <v>20190819</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B19" s="9">
         <v>20190920</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B20" s="9">
         <v>20190925</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B22" s="9">
         <v>20200201</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B23" s="9">
         <v>20220605</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B24" s="9">
         <v>20200704</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B25" s="9">
         <v>20201013</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B26" s="9">
         <v>20201028</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B28" s="9">
         <v>20210129</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B29" s="9">
         <v>20210329</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B31" s="9">
         <v>20210716</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B32" s="9">
         <v>20211026</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D33" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B34" s="9">
         <v>20211117</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B35" s="9">
         <v>20211126</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B36" s="9">
         <v>20220216</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B37" s="9">
         <v>20220408</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D38" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B39" s="9">
         <v>20220713</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B40" s="9">
         <v>20220729</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B41" s="9">
         <v>20220804</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B42" s="9">
         <v>20221109</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B44" s="9">
         <v>20230111</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2679,8 +2663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2698,7 +2682,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -2714,7 +2698,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -2722,7 +2706,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -2730,7 +2714,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -2746,7 +2730,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -2762,54 +2746,22 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update depth attribute definition
</commit_message>
<xml_diff>
--- a/chl-transect-info.xlsx
+++ b/chl-transect-info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-chl-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\nes-ims\nes-lter-chl-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B953B5-3280-4F31-A40B-78FB9F81D304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DAC945-7611-42F6-973A-0E0D4F40ABAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -361,9 +361,6 @@
     <t>iode_quality_flag</t>
   </si>
   <si>
-    <t>Depth of sample below sea surface as recorded by CTD</t>
-  </si>
-  <si>
     <t>IODE Quality Flag primary level</t>
   </si>
   <si>
@@ -647,13 +644,16 @@
   </si>
   <si>
     <t>OCE-2322676</t>
+  </si>
+  <si>
+    <t>Depth of sample below sea surface http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -705,6 +705,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -754,7 +760,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -778,6 +784,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1096,18 +1103,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.19921875" customWidth="1"/>
+    <col min="1" max="1" width="26.25" customWidth="1"/>
     <col min="2" max="2" width="65" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1141,7 +1148,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1152,7 +1159,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1163,7 +1170,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -1177,13 +1184,13 @@
         <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1197,13 +1204,13 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1217,18 +1224,18 @@
         <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
-        <v>110</v>
+      <c r="B8" s="11" t="s">
+        <v>205</v>
       </c>
       <c r="C8" t="s">
         <v>47</v>
@@ -1237,24 +1244,24 @@
         <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1265,7 +1272,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -1276,12 +1283,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>47</v>
@@ -1290,13 +1297,13 @@
         <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1310,35 +1317,35 @@
         <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1349,13 +1356,13 @@
         <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1369,7 +1376,7 @@
         <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G17" t="s">
         <v>102</v>
@@ -1388,14 +1395,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.3984375" customWidth="1"/>
-    <col min="2" max="2" width="24.8984375" customWidth="1"/>
-    <col min="3" max="3" width="21.69921875" customWidth="1"/>
+    <col min="1" max="1" width="24.375" customWidth="1"/>
+    <col min="2" max="2" width="24.875" customWidth="1"/>
+    <col min="3" max="3" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1413,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1428,7 +1435,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -1439,7 +1446,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -1461,7 +1468,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1472,95 +1479,95 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -1568,10 +1575,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -1579,10 +1586,10 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -1590,10 +1597,10 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -1601,10 +1608,10 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -1612,7 +1619,7 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1624,18 +1631,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.296875" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
-    <col min="7" max="7" width="14.296875" customWidth="1"/>
+    <col min="1" max="1" width="22.25" customWidth="1"/>
+    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="7" max="7" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1667,7 +1674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1696,15 +1703,15 @@
         <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -1713,10 +1720,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -1728,24 +1735,24 @@
         <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
         <v>132</v>
-      </c>
-      <c r="C4" t="s">
-        <v>133</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1757,10 +1764,10 @@
         <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -1786,24 +1793,24 @@
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
         <v>134</v>
-      </c>
-      <c r="C6" t="s">
-        <v>135</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
@@ -1815,10 +1822,10 @@
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1844,10 +1851,10 @@
         <v>24</v>
       </c>
       <c r="J7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1873,18 +1880,18 @@
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G9" t="s">
         <v>23</v>
@@ -1899,7 +1906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1928,10 +1935,10 @@
         <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -1957,10 +1964,10 @@
         <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -1986,21 +1993,21 @@
         <v>24</v>
       </c>
       <c r="J12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s">
         <v>137</v>
-      </c>
-      <c r="C13" t="s">
-        <v>138</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G13" t="s">
         <v>26</v>
@@ -2012,10 +2019,10 @@
         <v>24</v>
       </c>
       <c r="J13" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2066,39 +2073,39 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="9">
         <v>201704</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="B3" s="9">
         <v>20170902</v>
@@ -2107,12 +2114,12 @@
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" s="9">
         <v>20171022</v>
@@ -2121,36 +2128,36 @@
         <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" s="9">
         <v>20180131</v>
@@ -2159,12 +2166,12 @@
         <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="9">
         <v>20180404</v>
@@ -2173,24 +2180,24 @@
         <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" s="9">
         <v>20180720</v>
@@ -2199,12 +2206,12 @@
         <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="9">
         <v>20181020</v>
@@ -2213,36 +2220,36 @@
         <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B14" s="9">
         <v>20181112</v>
@@ -2251,12 +2258,12 @@
         <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" s="9">
         <v>20190201</v>
@@ -2265,12 +2272,12 @@
         <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B16" s="9">
         <v>20190414</v>
@@ -2279,24 +2286,24 @@
         <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B18" s="9">
         <v>20190819</v>
@@ -2305,12 +2312,12 @@
         <v>81</v>
       </c>
       <c r="D18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B19" s="9">
         <v>20190920</v>
@@ -2319,12 +2326,12 @@
         <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B20" s="9">
         <v>20190925</v>
@@ -2333,24 +2340,24 @@
         <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" s="9">
         <v>20200201</v>
@@ -2359,12 +2366,12 @@
         <v>81</v>
       </c>
       <c r="D22" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B23" s="9">
         <v>20220605</v>
@@ -2373,9 +2380,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B24" s="9">
         <v>20200704</v>
@@ -2384,12 +2391,12 @@
         <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B25" s="9">
         <v>20201013</v>
@@ -2398,12 +2405,12 @@
         <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B26" s="9">
         <v>20201028</v>
@@ -2412,18 +2419,18 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B28" s="9">
         <v>20210129</v>
@@ -2432,12 +2439,12 @@
         <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B29" s="9">
         <v>20210329</v>
@@ -2446,18 +2453,18 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B31" s="9">
         <v>20210716</v>
@@ -2466,12 +2473,12 @@
         <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B32" s="9">
         <v>20211026</v>
@@ -2480,32 +2487,32 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D33" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B34" s="9">
         <v>20211117</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B35" s="9">
         <v>20211126</v>
@@ -2514,9 +2521,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B36" s="9">
         <v>20220216</v>
@@ -2525,12 +2532,12 @@
         <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B37" s="9">
         <v>20220408</v>
@@ -2539,32 +2546,32 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D38" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B39" s="9">
         <v>20220713</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B40" s="9">
         <v>20220729</v>
@@ -2573,23 +2580,23 @@
         <v>81</v>
       </c>
       <c r="D40" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B41" s="9">
         <v>20220804</v>
       </c>
       <c r="C41" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="8" t="s">
-        <v>197</v>
       </c>
       <c r="B42" s="9">
         <v>20221109</v>
@@ -2598,18 +2605,18 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B44" s="9">
         <v>20230111</v>
@@ -2632,12 +2639,12 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2645,7 +2652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -2653,7 +2660,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2661,15 +2668,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>94</v>
       </c>
@@ -2677,7 +2684,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -2685,7 +2692,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
@@ -2693,7 +2700,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>96</v>
       </c>
@@ -2701,7 +2708,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
@@ -2709,7 +2716,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>98</v>
       </c>
@@ -2717,7 +2724,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>98</v>
       </c>

</xml_diff>